<commit_message>
Update 75+ D or F_Econ Disadv - Accountability Analysis_10.21.25.xlsx
</commit_message>
<xml_diff>
--- a/examples/75+ D or F_Econ Disadv - Accountability Analysis_10.21.25.xlsx
+++ b/examples/75+ D or F_Econ Disadv - Accountability Analysis_10.21.25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adpena/PycharmProjects/teadata/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51271459-27E2-F947-9D78-06734CD475C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF9DB89-DA2C-3E4E-BBB1-46E90E6AB81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8760" yWindow="620" windowWidth="20040" windowHeight="16260" xr2:uid="{32F109C2-AFD2-974A-B835-C347F758BC83}"/>
   </bookViews>
@@ -6797,7 +6797,18 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6878,16 +6889,19 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -6919,20 +6933,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6947,32 +6947,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F97984E-7812-6344-8B6E-5AAE396C4954}" name="DataTbl3" displayName="DataTbl3" ref="A1:P796" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="18" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F97984E-7812-6344-8B6E-5AAE396C4954}" name="DataTbl3" displayName="DataTbl3" ref="A1:P796" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A1:P796" xr:uid="{5F97984E-7812-6344-8B6E-5AAE396C4954}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{C0B9E6B1-9352-E240-9FF4-CBD47BEA4492}" name="Campus Number" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{C323DEAD-B42B-1F49-89DE-FBD68765B0D5}" name="Campus Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{4F8AE949-8845-874F-9DC7-AA1AC0D93F32}" name="District Name" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{3C3A644F-2326-7945-A9E4-6737C733786C}" name="County" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2FC5B167-7D9D-2447-897A-4DC276260AC9}" name="District/Charter" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{B18F425D-6D8F-4F4D-80FC-95401FFC2F6A}" name="Grades Served" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{FD76A1C1-2845-4840-A75E-976010B08464}" name="School Type" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{E6CB5202-DD25-7A44-B8C0-B7DFD69203BF}" name="Is Magnet" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{4A144A11-FD6F-A64F-B38D-B6C558F5B075}" name="2025 Overall Rating" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{8975AF02-63D5-424C-BC5E-B86E0160139C}" name="2023-24 % Economically Disadvantaged" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{9FE3250E-DE80-6646-AC78-8FBE8B075002}" name="2023-24 % Special Education" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{D7154193-4ED3-5F45-9120-B5FA25EBD294}" name="2023-24 % Attrition (2022-23)" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{2471F490-74BC-634D-8852-1F3BEE977BF6}" name="2023-24 % Mobility (2023)" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{2AD82158-3399-F74C-AEDD-DDE4401B3677}" name="2023-24 % At-Risk" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E0934E6F-C703-0F4F-BF3C-FEFFC878BB42}" name="2023-24 % Emergent Bilingual (EL)" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{9ECB4A7F-8F25-EA48-B703-244313F6B32F}" name="2023-24 % Beginning Teachers" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C0B9E6B1-9352-E240-9FF4-CBD47BEA4492}" name="Campus Number" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C323DEAD-B42B-1F49-89DE-FBD68765B0D5}" name="Campus Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4F8AE949-8845-874F-9DC7-AA1AC0D93F32}" name="District Name" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3C3A644F-2326-7945-A9E4-6737C733786C}" name="County" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{2FC5B167-7D9D-2447-897A-4DC276260AC9}" name="District/Charter" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B18F425D-6D8F-4F4D-80FC-95401FFC2F6A}" name="Grades Served" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{FD76A1C1-2845-4840-A75E-976010B08464}" name="School Type" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{E6CB5202-DD25-7A44-B8C0-B7DFD69203BF}" name="Is Magnet" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{4A144A11-FD6F-A64F-B38D-B6C558F5B075}" name="2025 Overall Rating" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{8975AF02-63D5-424C-BC5E-B86E0160139C}" name="2023-24 % Economically Disadvantaged" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{9FE3250E-DE80-6646-AC78-8FBE8B075002}" name="2023-24 % Special Education" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{D7154193-4ED3-5F45-9120-B5FA25EBD294}" name="2023-24 % Attrition (2022-23)" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{2471F490-74BC-634D-8852-1F3BEE977BF6}" name="2023-24 % Mobility (2023)" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{2AD82158-3399-F74C-AEDD-DDE4401B3677}" name="2023-24 % At-Risk" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{E0934E6F-C703-0F4F-BF3C-FEFFC878BB42}" name="2023-24 % Emergent Bilingual (EL)" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{9ECB4A7F-8F25-EA48-B703-244313F6B32F}" name="2023-24 % Beginning Teachers" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0EF880C-4285-5B42-97E1-D3C60FF59248}" name="DataTbl" displayName="DataTbl" ref="A1:P108" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0EF880C-4285-5B42-97E1-D3C60FF59248}" name="DataTbl" displayName="DataTbl" ref="A1:P108" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:P108" xr:uid="{D0EF880C-4285-5B42-97E1-D3C60FF59248}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{7BEB0BA1-1637-084C-8FB4-2C02396388F7}" name="Campus Number"/>
@@ -7319,7 +7319,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>